<commit_message>
Mejorando base de datos
</commit_message>
<xml_diff>
--- a/Datos/Datos_Wins.xlsx
+++ b/Datos/Datos_Wins.xlsx
@@ -636,7 +636,7 @@
   <dimension ref="A1:AB161"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1:T1048576"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7301,404 +7301,244 @@
       </c>
     </row>
     <row r="82" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="C82" s="1">
-        <v>1</v>
-      </c>
+      <c r="C82" s="1"/>
     </row>
     <row r="83" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="C83" s="1">
-        <v>2</v>
-      </c>
+      <c r="C83" s="1"/>
     </row>
     <row r="84" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="C84" s="1">
-        <v>3</v>
-      </c>
+      <c r="C84" s="1"/>
     </row>
     <row r="85" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="C85" s="1">
-        <v>4</v>
-      </c>
+      <c r="C85" s="1"/>
     </row>
     <row r="86" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="C86" s="1">
-        <v>5</v>
-      </c>
+      <c r="C86" s="1"/>
     </row>
     <row r="87" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="C87" s="1">
-        <v>6</v>
-      </c>
+      <c r="C87" s="1"/>
     </row>
     <row r="88" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="C88" s="1">
-        <v>7</v>
-      </c>
+      <c r="C88" s="1"/>
     </row>
     <row r="89" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="C89" s="1">
-        <v>8</v>
-      </c>
+      <c r="C89" s="1"/>
     </row>
     <row r="90" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="C90" s="1">
-        <v>1</v>
-      </c>
+      <c r="C90" s="1"/>
     </row>
     <row r="91" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="C91" s="1">
-        <v>2</v>
-      </c>
+      <c r="C91" s="1"/>
     </row>
     <row r="92" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="C92" s="1">
-        <v>3</v>
-      </c>
+      <c r="C92" s="1"/>
     </row>
     <row r="93" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="C93" s="1">
-        <v>4</v>
-      </c>
+      <c r="C93" s="1"/>
     </row>
     <row r="94" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="C94" s="1">
-        <v>5</v>
-      </c>
+      <c r="C94" s="1"/>
     </row>
     <row r="95" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="C95" s="1">
-        <v>6</v>
-      </c>
+      <c r="C95" s="1"/>
     </row>
     <row r="96" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="C96" s="1">
-        <v>7</v>
-      </c>
+      <c r="C96" s="1"/>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C97" s="1">
-        <v>8</v>
-      </c>
+      <c r="C97" s="1"/>
     </row>
     <row r="98" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C98" s="1">
-        <v>1</v>
-      </c>
+      <c r="C98" s="1"/>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C99" s="1">
-        <v>2</v>
-      </c>
+      <c r="C99" s="1"/>
     </row>
     <row r="100" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C100" s="1">
-        <v>3</v>
-      </c>
+      <c r="C100" s="1"/>
     </row>
     <row r="101" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C101" s="1">
-        <v>4</v>
-      </c>
+      <c r="C101" s="1"/>
     </row>
     <row r="102" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C102" s="1">
-        <v>5</v>
-      </c>
+      <c r="C102" s="1"/>
     </row>
     <row r="103" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C103" s="1">
-        <v>6</v>
-      </c>
+      <c r="C103" s="1"/>
     </row>
     <row r="104" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C104" s="1">
-        <v>7</v>
-      </c>
+      <c r="C104" s="1"/>
     </row>
     <row r="105" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C105" s="1">
-        <v>8</v>
-      </c>
+      <c r="C105" s="1"/>
     </row>
     <row r="106" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C106" s="1">
-        <v>1</v>
-      </c>
+      <c r="C106" s="1"/>
     </row>
     <row r="107" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C107" s="1">
-        <v>2</v>
-      </c>
+      <c r="C107" s="1"/>
     </row>
     <row r="108" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C108" s="1">
-        <v>3</v>
-      </c>
+      <c r="C108" s="1"/>
     </row>
     <row r="109" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C109" s="1">
-        <v>4</v>
-      </c>
+      <c r="C109" s="1"/>
     </row>
     <row r="110" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C110" s="1">
-        <v>5</v>
-      </c>
+      <c r="C110" s="1"/>
     </row>
     <row r="111" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C111" s="1">
-        <v>6</v>
-      </c>
+      <c r="C111" s="1"/>
     </row>
     <row r="112" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C112" s="1">
-        <v>7</v>
-      </c>
+      <c r="C112" s="1"/>
     </row>
     <row r="113" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C113" s="1">
-        <v>8</v>
-      </c>
+      <c r="C113" s="1"/>
     </row>
     <row r="114" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C114" s="1">
-        <v>1</v>
-      </c>
+      <c r="C114" s="1"/>
     </row>
     <row r="115" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C115" s="1">
-        <v>2</v>
-      </c>
+      <c r="C115" s="1"/>
     </row>
     <row r="116" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C116" s="1">
-        <v>3</v>
-      </c>
+      <c r="C116" s="1"/>
     </row>
     <row r="117" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C117" s="1">
-        <v>4</v>
-      </c>
+      <c r="C117" s="1"/>
     </row>
     <row r="118" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C118" s="1">
-        <v>5</v>
-      </c>
+      <c r="C118" s="1"/>
     </row>
     <row r="119" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C119" s="1">
-        <v>6</v>
-      </c>
+      <c r="C119" s="1"/>
     </row>
     <row r="120" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C120" s="1">
-        <v>7</v>
-      </c>
+      <c r="C120" s="1"/>
     </row>
     <row r="121" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C121" s="1">
-        <v>8</v>
-      </c>
+      <c r="C121" s="1"/>
     </row>
     <row r="122" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C122" s="1">
-        <v>1</v>
-      </c>
+      <c r="C122" s="1"/>
     </row>
     <row r="123" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C123" s="1">
-        <v>2</v>
-      </c>
+      <c r="C123" s="1"/>
     </row>
     <row r="124" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C124" s="1">
-        <v>3</v>
-      </c>
+      <c r="C124" s="1"/>
     </row>
     <row r="125" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C125" s="1">
-        <v>4</v>
-      </c>
+      <c r="C125" s="1"/>
     </row>
     <row r="126" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C126" s="1">
-        <v>5</v>
-      </c>
+      <c r="C126" s="1"/>
     </row>
     <row r="127" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C127" s="1">
-        <v>6</v>
-      </c>
+      <c r="C127" s="1"/>
     </row>
     <row r="128" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C128" s="1">
-        <v>7</v>
-      </c>
+      <c r="C128" s="1"/>
     </row>
     <row r="129" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C129" s="1">
-        <v>8</v>
-      </c>
+      <c r="C129" s="1"/>
     </row>
     <row r="130" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C130" s="1">
-        <v>1</v>
-      </c>
+      <c r="C130" s="1"/>
     </row>
     <row r="131" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C131" s="1">
-        <v>2</v>
-      </c>
+      <c r="C131" s="1"/>
     </row>
     <row r="132" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C132" s="1">
-        <v>3</v>
-      </c>
+      <c r="C132" s="1"/>
     </row>
     <row r="133" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C133" s="1">
-        <v>4</v>
-      </c>
+      <c r="C133" s="1"/>
     </row>
     <row r="134" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C134" s="1">
-        <v>5</v>
-      </c>
+      <c r="C134" s="1"/>
     </row>
     <row r="135" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C135" s="1">
-        <v>6</v>
-      </c>
+      <c r="C135" s="1"/>
     </row>
     <row r="136" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C136" s="1">
-        <v>7</v>
-      </c>
+      <c r="C136" s="1"/>
     </row>
     <row r="137" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C137" s="1">
-        <v>8</v>
-      </c>
+      <c r="C137" s="1"/>
     </row>
     <row r="138" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C138" s="1">
-        <v>1</v>
-      </c>
+      <c r="C138" s="1"/>
     </row>
     <row r="139" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C139" s="1">
-        <v>2</v>
-      </c>
+      <c r="C139" s="1"/>
     </row>
     <row r="140" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C140" s="1">
-        <v>3</v>
-      </c>
+      <c r="C140" s="1"/>
     </row>
     <row r="141" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C141" s="1">
-        <v>4</v>
-      </c>
+      <c r="C141" s="1"/>
     </row>
     <row r="142" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C142" s="1">
-        <v>5</v>
-      </c>
+      <c r="C142" s="1"/>
     </row>
     <row r="143" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C143" s="1">
-        <v>6</v>
-      </c>
+      <c r="C143" s="1"/>
     </row>
     <row r="144" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C144" s="1">
-        <v>7</v>
-      </c>
+      <c r="C144" s="1"/>
     </row>
     <row r="145" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C145" s="1">
-        <v>8</v>
-      </c>
+      <c r="C145" s="1"/>
     </row>
     <row r="146" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C146" s="1">
-        <v>1</v>
-      </c>
+      <c r="C146" s="1"/>
     </row>
     <row r="147" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C147" s="1">
-        <v>2</v>
-      </c>
+      <c r="C147" s="1"/>
     </row>
     <row r="148" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C148" s="1">
-        <v>3</v>
-      </c>
+      <c r="C148" s="1"/>
     </row>
     <row r="149" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C149" s="1">
-        <v>4</v>
-      </c>
+      <c r="C149" s="1"/>
     </row>
     <row r="150" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C150" s="1">
-        <v>5</v>
-      </c>
+      <c r="C150" s="1"/>
     </row>
     <row r="151" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C151" s="1">
-        <v>6</v>
-      </c>
+      <c r="C151" s="1"/>
     </row>
     <row r="152" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C152" s="1">
-        <v>7</v>
-      </c>
+      <c r="C152" s="1"/>
     </row>
     <row r="153" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C153" s="1">
-        <v>8</v>
-      </c>
+      <c r="C153" s="1"/>
     </row>
     <row r="154" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C154" s="1">
-        <v>1</v>
-      </c>
+      <c r="C154" s="1"/>
     </row>
     <row r="155" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C155" s="1">
-        <v>2</v>
-      </c>
+      <c r="C155" s="1"/>
     </row>
     <row r="156" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C156" s="1">
-        <v>3</v>
-      </c>
+      <c r="C156" s="1"/>
     </row>
     <row r="157" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C157" s="1">
-        <v>4</v>
-      </c>
+      <c r="C157" s="1"/>
     </row>
     <row r="158" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C158" s="1">
-        <v>5</v>
-      </c>
+      <c r="C158" s="1"/>
     </row>
     <row r="159" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C159" s="1">
-        <v>6</v>
-      </c>
+      <c r="C159" s="1"/>
     </row>
     <row r="160" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C160" s="1">
-        <v>7</v>
-      </c>
+      <c r="C160" s="1"/>
     </row>
     <row r="161" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C161" s="1">
-        <v>8</v>
-      </c>
+      <c r="C161" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>